<commit_message>
sighUp+purchase+cancellation and some restassured tests
</commit_message>
<xml_diff>
--- a/com.test.testAndroidMFP/users/users.xlsx
+++ b/com.test.testAndroidMFP/users/users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IdeaProjects\GitHub_tests\com.test.testAndroidMFP\users\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BAF42A-C06E-4D11-A1CC-CE15CC8438FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E47E616-7A15-4C50-97E4-C9C13EF99129}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13905" yWindow="5700" windowWidth="23025" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="4365" windowWidth="20760" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>UserName</t>
   </si>
@@ -36,31 +36,25 @@
     <t>Password</t>
   </si>
   <si>
-    <t>stranger495357</t>
-  </si>
-  <si>
-    <t>stranger495357@mail.com</t>
-  </si>
-  <si>
-    <t>1495357</t>
-  </si>
-  <si>
-    <t>str6298</t>
-  </si>
-  <si>
-    <t>str6298@mail.us</t>
-  </si>
-  <si>
-    <t>116298</t>
-  </si>
-  <si>
-    <t>sr517</t>
-  </si>
-  <si>
-    <t>s440@mail.com</t>
-  </si>
-  <si>
-    <t>111638</t>
+    <t>srxp7059</t>
+  </si>
+  <si>
+    <t>s662@mail.com</t>
+  </si>
+  <si>
+    <t>1111119928</t>
+  </si>
+  <si>
+    <t>srxp1171</t>
+  </si>
+  <si>
+    <t>s5633@mail.com</t>
+  </si>
+  <si>
+    <t>1111113</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -391,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,13 +411,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -435,17 +429,6 @@
       </c>
       <c r="C3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>